<commit_message>
Suppression du JDV localisation anatomique dans imagingStudy 98d143449efa2df9c379a584818d22089ac2c827
</commit_message>
<xml_diff>
--- a/majImagerie/ig/StructureDefinition-fr-imaging-study-document.xlsx
+++ b/majImagerie/ig/StructureDefinition-fr-imaging-study-document.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="458">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-05T10:47:15+00:00</t>
+    <t>2025-12-05T14:21:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1182,13 +1182,19 @@
 </t>
   </si>
   <si>
-    <t>Localisation anatomique</t>
+    <t>Localisation anatomique en SNOMED CT</t>
   </si>
   <si>
     <t>The anatomic structures examined. See DICOM Part 16 Annex L (http://dicom.nema.org/medical/dicom/current/output/chtml/part16/chapter_L.html) for DICOM to SNOMED-CT mappings. The bodySite may indicate the laterality of body part imaged; if so, it shall be consistent with any content of ImagingStudy.series.laterality.</t>
   </si>
   <si>
-    <t>https://smt.esante.gouv.fr/fhir/ValueSet/jdv-localisation-anatomique-cisis</t>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes describing anatomical locations. May include laterality.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/body-site|4.0.1</t>
   </si>
   <si>
     <t>.targetSiteCode</t>
@@ -1799,7 +1805,7 @@
     <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="34.12109375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="49.63671875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="61.59375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
@@ -6590,7 +6596,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
         <v>368</v>
       </c>
@@ -6603,13 +6609,13 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>89</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="I42" t="s" s="2">
         <v>78</v>
@@ -6651,11 +6657,13 @@
         <v>78</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="Y42" s="2"/>
+        <v>372</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="Z42" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>78</v>
@@ -6691,10 +6699,10 @@
         <v>78</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>78</v>
@@ -6705,10 +6713,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6734,10 +6742,10 @@
         <v>176</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6768,7 +6776,7 @@
       </c>
       <c r="Y43" s="2"/>
       <c r="Z43" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>78</v>
@@ -6786,7 +6794,7 @@
         <v>78</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -6804,10 +6812,10 @@
         <v>78</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>78</v>
@@ -6818,10 +6826,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6844,13 +6852,13 @@
         <v>90</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6901,7 +6909,7 @@
         <v>78</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -6919,10 +6927,10 @@
         <v>78</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>78</v>
@@ -6933,10 +6941,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6962,10 +6970,10 @@
         <v>202</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7016,7 +7024,7 @@
         <v>78</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -7037,7 +7045,7 @@
         <v>207</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>78</v>
@@ -7048,14 +7056,14 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -7077,16 +7085,16 @@
         <v>313</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="O46" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="P46" t="s" s="2">
         <v>78</v>
@@ -7135,7 +7143,7 @@
         <v>78</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7150,13 +7158,13 @@
         <v>101</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>235</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>78</v>
@@ -7167,10 +7175,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7282,10 +7290,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7399,10 +7407,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7518,10 +7526,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7547,14 +7555,14 @@
         <v>267</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>78</v>
@@ -7582,10 +7590,10 @@
         <v>270</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>78</v>
@@ -7603,7 +7611,7 @@
         <v>78</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -7635,10 +7643,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7661,13 +7669,13 @@
         <v>90</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7718,7 +7726,7 @@
         <v>78</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>89</v>
@@ -7736,24 +7744,24 @@
         <v>78</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7779,10 +7787,10 @@
         <v>313</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7833,7 +7841,7 @@
         <v>78</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>79</v>
@@ -7851,7 +7859,7 @@
         <v>78</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>78</v>
@@ -7865,10 +7873,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7980,10 +7988,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8009,10 +8017,10 @@
         <v>135</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -8051,7 +8059,7 @@
         <v>78</v>
       </c>
       <c r="AB54" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AC54" s="2"/>
       <c r="AD54" t="s" s="2">
@@ -8093,13 +8101,13 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D55" t="s" s="2">
         <v>78</v>
@@ -8121,13 +8129,13 @@
         <v>78</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8187,7 +8195,7 @@
         <v>80</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>140</v>
@@ -8210,10 +8218,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8329,14 +8337,14 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -8358,16 +8366,16 @@
         <v>91</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="O57" t="s" s="2">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="P57" t="s" s="2">
         <v>78</v>
@@ -8380,7 +8388,7 @@
         <v>78</v>
       </c>
       <c r="T57" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="U57" t="s" s="2">
         <v>78</v>
@@ -8416,7 +8424,7 @@
         <v>78</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>89</v>
@@ -8437,7 +8445,7 @@
         <v>337</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>78</v>
@@ -8448,14 +8456,14 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -8477,10 +8485,10 @@
         <v>176</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8511,7 +8519,7 @@
       </c>
       <c r="Y58" s="2"/>
       <c r="Z58" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AA58" t="s" s="2">
         <v>78</v>
@@ -8529,7 +8537,7 @@
         <v>78</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>89</v>
@@ -8547,10 +8555,10 @@
         <v>78</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>78</v>
@@ -8561,14 +8569,14 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
@@ -8590,10 +8598,10 @@
         <v>247</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8644,7 +8652,7 @@
         <v>78</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>79</v>
@@ -8662,10 +8670,10 @@
         <v>78</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>78</v>
@@ -8676,10 +8684,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8705,13 +8713,13 @@
         <v>307</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -8761,7 +8769,7 @@
         <v>78</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>79</v>
@@ -8779,10 +8787,10 @@
         <v>78</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>78</v>

</xml_diff>